<commit_message>
20250116 device object size
</commit_message>
<xml_diff>
--- a/casual1/Assets/Resources/GradeDB.xlsx
+++ b/casual1/Assets/Resources/GradeDB.xlsx
@@ -456,7 +456,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -532,10 +532,10 @@
         <v>16</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
20250210 start scene change
</commit_message>
<xml_diff>
--- a/casual1/Assets/Resources/GradeDB.xlsx
+++ b/casual1/Assets/Resources/GradeDB.xlsx
@@ -456,7 +456,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -618,7 +618,7 @@
         <v>151</v>
       </c>
       <c r="D7">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>20</v>
@@ -638,10 +638,10 @@
         <v>12</v>
       </c>
       <c r="C8">
-        <v>201</v>
+        <v>251</v>
       </c>
       <c r="D8">
-        <v>300</v>
+        <v>350</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>21</v>
@@ -661,10 +661,10 @@
         <v>13</v>
       </c>
       <c r="C9">
-        <v>301</v>
+        <v>351</v>
       </c>
       <c r="D9">
-        <v>400</v>
+        <v>500</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>22</v>
@@ -684,10 +684,10 @@
         <v>14</v>
       </c>
       <c r="C10">
-        <v>401</v>
+        <v>501</v>
       </c>
       <c r="D10">
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>23</v>
@@ -707,7 +707,7 @@
         <v>15</v>
       </c>
       <c r="C11">
-        <v>501</v>
+        <v>801</v>
       </c>
       <c r="D11">
         <v>9999</v>

</xml_diff>